<commit_message>
selected covariates for waist.circ.
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/n ~4000/Div/10_Div Grouping.xlsx
+++ b/eg_data/NHANES/PF/n ~4000/Div/10_Div Grouping.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\n ~4000\Div\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12583D7E-2A78-46D4-BC46-9246BB517740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDA6E1C-D279-4503-9361-36D50D95AAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25410" yWindow="435" windowWidth="14100" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20880" yWindow="-2985" windowWidth="17910" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -436,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,12 +460,12 @@
     <col min="5" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -469,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -485,8 +496,12 @@
       <c r="F4" s="4">
         <v>406</v>
       </c>
+      <c r="G4">
+        <f>SUM(C4:F4)</f>
+        <v>4207</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -503,7 +518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -520,7 +535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>

</xml_diff>